<commit_message>
Úprava dokumentace podle připomínek z konzultace
</commit_message>
<xml_diff>
--- a/Dokumentace/benchmark-results.xlsx
+++ b/Dokumentace/benchmark-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\diplomka\Dokumentace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177ACB76-DC95-4F2C-99F9-BACE1EF412C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299CC7F-0B8F-41C2-916C-6601B07B268C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{209728F2-C094-423C-80BE-A506D0BCB5A3}"/>
   </bookViews>
@@ -942,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1027,16 +1027,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1056,6 +1056,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1373,23 +1376,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3950500D-10BC-4704-8A46-A63808D85E74}">
   <dimension ref="C3:AN482"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I40"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P140" sqref="P140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="1"/>
     <col min="11" max="11" width="49.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.44140625" style="1" customWidth="1"/>
@@ -1601,16 +1604,16 @@
     </row>
     <row r="6" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="39"/>
       <c r="L6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2382,14 +2385,14 @@
     </row>
     <row r="17" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C17" s="7"/>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
       <c r="L17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2465,16 +2468,16 @@
     </row>
     <row r="18" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C18" s="7"/>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36" t="s">
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
       <c r="L18" s="1" t="s">
         <v>18</v>
       </c>
@@ -3282,14 +3285,14 @@
     </row>
     <row r="29" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C29" s="7"/>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39"/>
       <c r="L29" s="1" t="s">
         <v>26</v>
       </c>
@@ -3365,16 +3368,16 @@
     </row>
     <row r="30" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C30" s="7"/>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36" t="s">
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="39"/>
       <c r="L30" s="1" t="s">
         <v>9</v>
       </c>
@@ -4348,16 +4351,16 @@
     </row>
     <row r="44" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C44" s="7"/>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36" t="s">
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="39"/>
       <c r="L44" s="1" t="s">
         <v>34</v>
       </c>
@@ -5669,14 +5672,14 @@
     </row>
     <row r="60" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C60" s="7"/>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="39"/>
       <c r="L60" s="1" t="s">
         <v>46</v>
       </c>
@@ -5752,16 +5755,16 @@
     </row>
     <row r="61" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C61" s="7"/>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36" t="s">
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="39"/>
       <c r="L61" s="1" t="s">
         <v>47</v>
       </c>
@@ -7062,14 +7065,14 @@
     </row>
     <row r="77" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C77" s="7"/>
-      <c r="D77" s="36" t="s">
+      <c r="D77" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="37"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="39"/>
       <c r="L77" s="1" t="s">
         <v>9</v>
       </c>
@@ -7127,16 +7130,16 @@
     </row>
     <row r="78" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C78" s="7"/>
-      <c r="D78" s="36" t="s">
+      <c r="D78" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36" t="s">
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H78" s="36"/>
-      <c r="I78" s="37"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="39"/>
       <c r="L78" s="1" t="s">
         <v>58</v>
       </c>
@@ -8511,14 +8514,14 @@
     </row>
     <row r="95" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C95" s="6"/>
-      <c r="D95" s="40" t="s">
+      <c r="D95" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E95" s="41"/>
-      <c r="F95" s="41"/>
-      <c r="G95" s="41"/>
-      <c r="H95" s="41"/>
-      <c r="I95" s="42"/>
+      <c r="E95" s="36"/>
+      <c r="F95" s="36"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="36"/>
+      <c r="I95" s="37"/>
       <c r="L95" s="1" t="s">
         <v>9</v>
       </c>
@@ -8576,16 +8579,16 @@
     </row>
     <row r="96" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C96" s="7"/>
-      <c r="D96" s="36" t="s">
+      <c r="D96" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36" t="s">
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H96" s="36"/>
-      <c r="I96" s="37"/>
+      <c r="H96" s="38"/>
+      <c r="I96" s="39"/>
       <c r="L96" s="1" t="s">
         <v>33</v>
       </c>
@@ -8751,14 +8754,14 @@
     </row>
     <row r="98" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C98" s="7"/>
-      <c r="D98" s="31" t="s">
+      <c r="D98" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="32"/>
-      <c r="I98" s="33"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+      <c r="I98" s="35"/>
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
       <c r="S98" s="5"/>
@@ -8785,14 +8788,14 @@
       <c r="F99" s="20">
         <v>7.6729900000000002E-3</v>
       </c>
-      <c r="G99" s="8">
-        <v>298667</v>
-      </c>
-      <c r="H99" s="9">
-        <v>2.37002E-3</v>
-      </c>
-      <c r="I99" s="10">
-        <v>2.40653E-3</v>
+      <c r="G99" s="19">
+        <v>344615</v>
+      </c>
+      <c r="H99" s="20">
+        <v>1.96605E-3</v>
+      </c>
+      <c r="I99" s="21">
+        <v>1.9949799999999999E-3</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>36</v>
@@ -8880,14 +8883,14 @@
       <c r="F100" s="20">
         <v>7.6729900000000002E-3</v>
       </c>
-      <c r="G100" s="8">
-        <v>280000</v>
-      </c>
-      <c r="H100" s="9">
-        <v>2.3860499999999998E-3</v>
-      </c>
-      <c r="I100" s="10">
-        <v>2.3437499999999999E-3</v>
+      <c r="G100" s="19">
+        <v>298667</v>
+      </c>
+      <c r="H100" s="20">
+        <v>2.2800199999999998E-3</v>
+      </c>
+      <c r="I100" s="21">
+        <v>2.30189E-3</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>71</v>
@@ -8964,14 +8967,14 @@
     </row>
     <row r="101" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C101" s="18"/>
-      <c r="D101" s="31" t="s">
+      <c r="D101" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="33"/>
+      <c r="E101" s="34"/>
+      <c r="F101" s="34"/>
+      <c r="G101" s="34"/>
+      <c r="H101" s="34"/>
+      <c r="I101" s="35"/>
       <c r="N101" s="5"/>
       <c r="O101" s="5"/>
       <c r="S101" s="5"/>
@@ -8998,14 +9001,14 @@
       <c r="F102" s="20">
         <v>0.112305</v>
       </c>
-      <c r="G102" s="8">
-        <v>20364</v>
-      </c>
-      <c r="H102" s="9">
-        <v>3.51396E-2</v>
-      </c>
-      <c r="I102" s="10">
-        <v>3.3760600000000002E-2</v>
+      <c r="G102" s="19">
+        <v>19478</v>
+      </c>
+      <c r="H102" s="20">
+        <v>3.53558E-2</v>
+      </c>
+      <c r="I102" s="21">
+        <v>3.52962E-2</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>39</v>
@@ -9093,14 +9096,14 @@
       <c r="F103" s="20">
         <v>0.117188</v>
       </c>
-      <c r="G103" s="8">
-        <v>20364</v>
-      </c>
-      <c r="H103" s="9">
-        <v>3.4777700000000002E-2</v>
-      </c>
-      <c r="I103" s="10">
-        <v>3.5295100000000003E-2</v>
+      <c r="G103" s="19">
+        <v>22400</v>
+      </c>
+      <c r="H103" s="20">
+        <v>3.2005499999999999E-2</v>
+      </c>
+      <c r="I103" s="21">
+        <v>3.20871E-2</v>
       </c>
       <c r="L103" s="1" t="s">
         <v>72</v>
@@ -9177,14 +9180,14 @@
     </row>
     <row r="104" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C104" s="18"/>
-      <c r="D104" s="31" t="s">
+      <c r="D104" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E104" s="32"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="32"/>
-      <c r="H104" s="32"/>
-      <c r="I104" s="33"/>
+      <c r="E104" s="34"/>
+      <c r="F104" s="34"/>
+      <c r="G104" s="34"/>
+      <c r="H104" s="34"/>
+      <c r="I104" s="35"/>
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
       <c r="S104" s="5"/>
@@ -9211,14 +9214,14 @@
       <c r="F105" s="20">
         <v>5.6640600000000001</v>
       </c>
-      <c r="G105" s="8">
-        <v>747</v>
-      </c>
-      <c r="H105" s="9">
-        <v>1.0526599999999999</v>
-      </c>
-      <c r="I105" s="10">
-        <v>1.0458499999999999</v>
+      <c r="G105" s="19">
+        <v>264</v>
+      </c>
+      <c r="H105" s="20">
+        <v>2.6824300000000001</v>
+      </c>
+      <c r="I105" s="21">
+        <v>2.6633499999999999</v>
       </c>
       <c r="L105" s="1" t="s">
         <v>9</v>
@@ -9291,14 +9294,14 @@
       <c r="F106" s="20">
         <v>5.15625</v>
       </c>
-      <c r="G106" s="8">
-        <v>448</v>
-      </c>
-      <c r="H106" s="9">
-        <v>1.5171300000000001</v>
-      </c>
-      <c r="I106" s="10">
-        <v>1.5346</v>
+      <c r="G106" s="19">
+        <v>299</v>
+      </c>
+      <c r="H106" s="20">
+        <v>3.18058</v>
+      </c>
+      <c r="I106" s="21">
+        <v>3.18771</v>
       </c>
       <c r="L106" s="1" t="s">
         <v>73</v>
@@ -9360,14 +9363,14 @@
     </row>
     <row r="107" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C107" s="18"/>
-      <c r="D107" s="36" t="s">
+      <c r="D107" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E107" s="36"/>
-      <c r="F107" s="36"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="36"/>
-      <c r="I107" s="37"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="38"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="39"/>
       <c r="L107" s="1" t="s">
         <v>74</v>
       </c>
@@ -9440,16 +9443,16 @@
     </row>
     <row r="108" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C108" s="18"/>
-      <c r="D108" s="36" t="s">
+      <c r="D108" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="36"/>
-      <c r="F108" s="36"/>
-      <c r="G108" s="36" t="s">
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H108" s="36"/>
-      <c r="I108" s="37"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="39"/>
       <c r="L108" s="1" t="s">
         <v>75</v>
       </c>
@@ -9618,14 +9621,14 @@
     </row>
     <row r="110" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C110" s="18"/>
-      <c r="D110" s="31" t="s">
+      <c r="D110" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="32"/>
-      <c r="H110" s="32"/>
-      <c r="I110" s="33"/>
+      <c r="E110" s="34"/>
+      <c r="F110" s="34"/>
+      <c r="G110" s="34"/>
+      <c r="H110" s="34"/>
+      <c r="I110" s="35"/>
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
       <c r="S110" s="5"/>
@@ -9643,23 +9646,23 @@
       <c r="C111" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D111" s="8">
-        <v>100000</v>
-      </c>
-      <c r="E111" s="9">
-        <v>5.4906800000000004E-3</v>
-      </c>
-      <c r="F111" s="9">
-        <v>5.6249999999999998E-3</v>
-      </c>
-      <c r="G111" s="8">
-        <v>280000</v>
-      </c>
-      <c r="H111" s="9">
-        <v>2.3876100000000001E-3</v>
-      </c>
-      <c r="I111" s="10">
-        <v>2.3437499999999999E-3</v>
+      <c r="D111" s="19">
+        <v>89600</v>
+      </c>
+      <c r="E111" s="20">
+        <v>7.7582800000000002E-3</v>
+      </c>
+      <c r="F111" s="20">
+        <v>7.6729900000000002E-3</v>
+      </c>
+      <c r="G111" s="19">
+        <v>320000</v>
+      </c>
+      <c r="H111" s="20">
+        <v>2.1337000000000001E-3</v>
+      </c>
+      <c r="I111" s="21">
+        <v>2.1484400000000002E-3</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>77</v>
@@ -9738,23 +9741,23 @@
       <c r="C112" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D112" s="8">
-        <v>100000</v>
-      </c>
-      <c r="E112" s="9">
-        <v>5.4596999999999996E-3</v>
-      </c>
-      <c r="F112" s="9">
-        <v>5.4687499999999997E-3</v>
-      </c>
-      <c r="G112" s="8">
-        <v>280000</v>
-      </c>
-      <c r="H112" s="9">
-        <v>2.4300699999999999E-3</v>
-      </c>
-      <c r="I112" s="10">
-        <v>2.3995499999999999E-3</v>
+      <c r="D112" s="19">
+        <v>89600</v>
+      </c>
+      <c r="E112" s="20">
+        <v>7.8757500000000008E-3</v>
+      </c>
+      <c r="F112" s="20">
+        <v>7.8473799999999993E-3</v>
+      </c>
+      <c r="G112" s="19">
+        <v>320000</v>
+      </c>
+      <c r="H112" s="20">
+        <v>2.1280800000000001E-3</v>
+      </c>
+      <c r="I112" s="21">
+        <v>2.09961E-3</v>
       </c>
       <c r="L112" s="1" t="s">
         <v>78</v>
@@ -9831,14 +9834,14 @@
     </row>
     <row r="113" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C113" s="18"/>
-      <c r="D113" s="31" t="s">
+      <c r="D113" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="32"/>
-      <c r="H113" s="32"/>
-      <c r="I113" s="33"/>
+      <c r="E113" s="34"/>
+      <c r="F113" s="34"/>
+      <c r="G113" s="34"/>
+      <c r="H113" s="34"/>
+      <c r="I113" s="35"/>
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
       <c r="S113" s="5"/>
@@ -9856,23 +9859,23 @@
       <c r="C114" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D114" s="8">
-        <v>8960</v>
-      </c>
-      <c r="E114" s="9">
-        <v>7.9068200000000005E-2</v>
-      </c>
-      <c r="F114" s="9">
-        <v>7.6729900000000004E-2</v>
-      </c>
-      <c r="G114" s="8">
-        <v>17231</v>
-      </c>
-      <c r="H114" s="9">
-        <v>3.6204800000000002E-2</v>
-      </c>
-      <c r="I114" s="10">
-        <v>3.5365000000000001E-2</v>
+      <c r="D114" s="19">
+        <v>4480</v>
+      </c>
+      <c r="E114" s="20">
+        <v>0.124237</v>
+      </c>
+      <c r="F114" s="20">
+        <v>0.125558</v>
+      </c>
+      <c r="G114" s="19">
+        <v>22400</v>
+      </c>
+      <c r="H114" s="20">
+        <v>3.2281400000000002E-2</v>
+      </c>
+      <c r="I114" s="21">
+        <v>3.20871E-2</v>
       </c>
       <c r="L114" s="1" t="s">
         <v>9</v>
@@ -9948,23 +9951,23 @@
       <c r="C115" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D115" s="8">
-        <v>8960</v>
-      </c>
-      <c r="E115" s="9">
-        <v>8.4000400000000003E-2</v>
-      </c>
-      <c r="F115" s="9">
-        <v>8.02176E-2</v>
-      </c>
-      <c r="G115" s="8">
+      <c r="D115" s="19">
+        <v>6400</v>
+      </c>
+      <c r="E115" s="20">
+        <v>0.13211500000000001</v>
+      </c>
+      <c r="F115" s="20">
+        <v>0.13183600000000001</v>
+      </c>
+      <c r="G115" s="19">
         <v>19478</v>
       </c>
-      <c r="H115" s="9">
-        <v>3.7782999999999997E-2</v>
-      </c>
-      <c r="I115" s="10">
-        <v>3.7702800000000002E-2</v>
+      <c r="H115" s="20">
+        <v>3.4192699999999999E-2</v>
+      </c>
+      <c r="I115" s="21">
+        <v>3.3691899999999997E-2</v>
       </c>
       <c r="L115" s="1" t="s">
         <v>9</v>
@@ -10026,14 +10029,14 @@
     </row>
     <row r="116" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C116" s="18"/>
-      <c r="D116" s="31" t="s">
+      <c r="D116" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="32"/>
-      <c r="H116" s="32"/>
-      <c r="I116" s="33"/>
+      <c r="E116" s="34"/>
+      <c r="F116" s="34"/>
+      <c r="G116" s="34"/>
+      <c r="H116" s="34"/>
+      <c r="I116" s="35"/>
       <c r="N116" s="5"/>
       <c r="O116" s="5"/>
       <c r="S116" s="5"/>
@@ -10051,23 +10054,23 @@
       <c r="C117" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D117" s="8">
-        <v>299</v>
-      </c>
-      <c r="E117" s="9">
-        <v>2.3091900000000001</v>
-      </c>
-      <c r="F117" s="9">
-        <v>2.2993299999999999</v>
-      </c>
-      <c r="G117" s="8">
-        <v>640</v>
-      </c>
-      <c r="H117" s="9">
-        <v>1.19834</v>
-      </c>
-      <c r="I117" s="10">
-        <v>1.1962900000000001</v>
+      <c r="D117" s="19">
+        <v>160</v>
+      </c>
+      <c r="E117" s="20">
+        <v>4.3853999999999997</v>
+      </c>
+      <c r="F117" s="20">
+        <v>4.3945299999999996</v>
+      </c>
+      <c r="G117" s="19">
+        <v>166</v>
+      </c>
+      <c r="H117" s="20">
+        <v>3.90442</v>
+      </c>
+      <c r="I117" s="21">
+        <v>3.8591899999999999</v>
       </c>
       <c r="L117" s="1" t="s">
         <v>79</v>
@@ -10131,23 +10134,23 @@
       <c r="C118" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D118" s="8">
-        <v>160</v>
-      </c>
-      <c r="E118" s="9">
-        <v>4.9169299999999998</v>
-      </c>
-      <c r="F118" s="9">
-        <v>4.8828100000000001</v>
-      </c>
-      <c r="G118" s="8">
-        <v>448</v>
-      </c>
-      <c r="H118" s="9">
-        <v>1.6133299999999999</v>
-      </c>
-      <c r="I118" s="10">
-        <v>1.63923</v>
+      <c r="D118" s="19">
+        <v>172</v>
+      </c>
+      <c r="E118" s="20">
+        <v>4.7112800000000004</v>
+      </c>
+      <c r="F118" s="20">
+        <v>4.72384</v>
+      </c>
+      <c r="G118" s="19">
+        <v>249</v>
+      </c>
+      <c r="H118" s="20">
+        <v>2.5510999999999999</v>
+      </c>
+      <c r="I118" s="21">
+        <v>2.5727899999999999</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>80</v>
@@ -10221,14 +10224,14 @@
     </row>
     <row r="119" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C119" s="18"/>
-      <c r="D119" s="36" t="s">
+      <c r="D119" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E119" s="36"/>
-      <c r="F119" s="36"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="36"/>
-      <c r="I119" s="37"/>
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
+      <c r="G119" s="38"/>
+      <c r="H119" s="38"/>
+      <c r="I119" s="39"/>
       <c r="L119" s="1" t="s">
         <v>81</v>
       </c>
@@ -10304,16 +10307,16 @@
     </row>
     <row r="120" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C120" s="18"/>
-      <c r="D120" s="36" t="s">
+      <c r="D120" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E120" s="36"/>
-      <c r="F120" s="36"/>
-      <c r="G120" s="36" t="s">
+      <c r="E120" s="38"/>
+      <c r="F120" s="38"/>
+      <c r="G120" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H120" s="36"/>
-      <c r="I120" s="37"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="39"/>
       <c r="L120" s="1" t="s">
         <v>82</v>
       </c>
@@ -10482,14 +10485,14 @@
     </row>
     <row r="122" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C122" s="18"/>
-      <c r="D122" s="31" t="s">
+      <c r="D122" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="32"/>
-      <c r="H122" s="32"/>
-      <c r="I122" s="33"/>
+      <c r="E122" s="34"/>
+      <c r="F122" s="34"/>
+      <c r="G122" s="34"/>
+      <c r="H122" s="34"/>
+      <c r="I122" s="35"/>
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
       <c r="S122" s="5"/>
@@ -10507,23 +10510,23 @@
       <c r="C123" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="8">
-        <v>100000</v>
-      </c>
-      <c r="E123" s="9">
-        <v>5.5139300000000002E-3</v>
-      </c>
-      <c r="F123" s="9">
-        <v>5.4687499999999997E-3</v>
-      </c>
-      <c r="G123" s="8">
-        <v>298667</v>
-      </c>
-      <c r="H123" s="9">
-        <v>2.3864200000000002E-3</v>
-      </c>
-      <c r="I123" s="10">
-        <v>2.3542099999999998E-3</v>
+      <c r="D123" s="19">
+        <v>89600</v>
+      </c>
+      <c r="E123" s="20">
+        <v>7.3079399999999997E-3</v>
+      </c>
+      <c r="F123" s="20">
+        <v>7.3242200000000002E-3</v>
+      </c>
+      <c r="G123" s="19">
+        <v>407273</v>
+      </c>
+      <c r="H123" s="20">
+        <v>1.7385199999999999E-3</v>
+      </c>
+      <c r="I123" s="21">
+        <v>1.72642E-3</v>
       </c>
       <c r="L123" s="1" t="s">
         <v>84</v>
@@ -10602,23 +10605,23 @@
       <c r="C124" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D124" s="8">
-        <v>112000</v>
-      </c>
-      <c r="E124" s="9">
-        <v>5.4807199999999997E-3</v>
-      </c>
-      <c r="F124" s="9">
-        <v>5.4408499999999997E-3</v>
-      </c>
-      <c r="G124" s="8">
-        <v>298667</v>
-      </c>
-      <c r="H124" s="9">
-        <v>2.39602E-3</v>
-      </c>
-      <c r="I124" s="10">
-        <v>2.40653E-3</v>
+      <c r="D124" s="19">
+        <v>89600</v>
+      </c>
+      <c r="E124" s="20">
+        <v>8.18142E-3</v>
+      </c>
+      <c r="F124" s="20">
+        <v>8.1961499999999993E-3</v>
+      </c>
+      <c r="G124" s="19">
+        <v>373333</v>
+      </c>
+      <c r="H124" s="20">
+        <v>1.8777100000000001E-3</v>
+      </c>
+      <c r="I124" s="21">
+        <v>1.8833700000000001E-3</v>
       </c>
       <c r="L124" s="1" t="s">
         <v>85</v>
@@ -10695,14 +10698,14 @@
     </row>
     <row r="125" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C125" s="18"/>
-      <c r="D125" s="31" t="s">
+      <c r="D125" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="E125" s="32"/>
-      <c r="F125" s="32"/>
-      <c r="G125" s="32"/>
-      <c r="H125" s="32"/>
-      <c r="I125" s="33"/>
+      <c r="E125" s="34"/>
+      <c r="F125" s="34"/>
+      <c r="G125" s="34"/>
+      <c r="H125" s="34"/>
+      <c r="I125" s="35"/>
       <c r="N125" s="5"/>
       <c r="O125" s="5"/>
       <c r="S125" s="5"/>
@@ -10720,23 +10723,23 @@
       <c r="C126" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D126" s="8">
-        <v>8960</v>
-      </c>
-      <c r="E126" s="9">
-        <v>7.8666799999999995E-2</v>
-      </c>
-      <c r="F126" s="9">
-        <v>7.8473799999999996E-2</v>
-      </c>
-      <c r="G126" s="8">
-        <v>19478</v>
-      </c>
-      <c r="H126" s="9">
-        <v>3.47564E-2</v>
-      </c>
-      <c r="I126" s="10">
-        <v>3.4493999999999997E-2</v>
+      <c r="D126" s="19">
+        <v>6400</v>
+      </c>
+      <c r="E126" s="20">
+        <v>0.11236400000000001</v>
+      </c>
+      <c r="F126" s="20">
+        <v>0.114746</v>
+      </c>
+      <c r="G126" s="19">
+        <v>23579</v>
+      </c>
+      <c r="H126" s="20">
+        <v>3.2772599999999999E-2</v>
+      </c>
+      <c r="I126" s="21">
+        <v>3.2470600000000002E-2</v>
       </c>
       <c r="L126" s="1" t="s">
         <v>86</v>
@@ -10815,23 +10818,23 @@
       <c r="C127" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D127" s="8">
-        <v>8960</v>
-      </c>
-      <c r="E127" s="9">
-        <v>7.8929100000000002E-2</v>
-      </c>
-      <c r="F127" s="9">
-        <v>7.8473799999999996E-2</v>
-      </c>
-      <c r="G127" s="8">
-        <v>20364</v>
-      </c>
-      <c r="H127" s="9">
-        <v>3.5150099999999997E-2</v>
-      </c>
-      <c r="I127" s="10">
-        <v>3.5295100000000003E-2</v>
+      <c r="D127" s="19">
+        <v>6400</v>
+      </c>
+      <c r="E127" s="20">
+        <v>0.112317</v>
+      </c>
+      <c r="F127" s="20">
+        <v>0.112305</v>
+      </c>
+      <c r="G127" s="19">
+        <v>23579</v>
+      </c>
+      <c r="H127" s="20">
+        <v>3.3748899999999998E-2</v>
+      </c>
+      <c r="I127" s="21">
+        <v>3.3796E-2</v>
       </c>
       <c r="L127" s="1" t="s">
         <v>87</v>
@@ -10906,16 +10909,16 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="128" spans="3:40" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C128" s="18"/>
-      <c r="D128" s="31" t="s">
+      <c r="D128" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E128" s="32"/>
-      <c r="F128" s="32"/>
-      <c r="G128" s="32"/>
-      <c r="H128" s="32"/>
-      <c r="I128" s="33"/>
+      <c r="E128" s="34"/>
+      <c r="F128" s="34"/>
+      <c r="G128" s="34"/>
+      <c r="H128" s="34"/>
+      <c r="I128" s="35"/>
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
       <c r="S128" s="5"/>
@@ -10933,23 +10936,23 @@
       <c r="C129" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D129" s="8">
-        <v>299</v>
-      </c>
-      <c r="E129" s="9">
-        <v>2.2919299999999998</v>
-      </c>
-      <c r="F129" s="9">
-        <v>2.2993299999999999</v>
-      </c>
-      <c r="G129" s="8">
-        <v>640</v>
-      </c>
-      <c r="H129" s="9">
-        <v>1.0400199999999999</v>
-      </c>
-      <c r="I129" s="10">
-        <v>1.02539</v>
+      <c r="D129" s="19">
+        <v>179</v>
+      </c>
+      <c r="E129" s="20">
+        <v>4.0296099999999999</v>
+      </c>
+      <c r="F129" s="20">
+        <v>4.1026499999999997</v>
+      </c>
+      <c r="G129" s="19">
+        <v>280</v>
+      </c>
+      <c r="H129" s="20">
+        <v>2.9904199999999999</v>
+      </c>
+      <c r="I129" s="21">
+        <v>2.9575900000000002</v>
       </c>
       <c r="L129" s="1" t="s">
         <v>9</v>
@@ -11022,26 +11025,26 @@
       </c>
     </row>
     <row r="130" spans="3:40" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C130" s="18" t="s">
+      <c r="C130" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="D130" s="12">
-        <v>160</v>
-      </c>
-      <c r="E130" s="13">
-        <v>4.3498799999999997</v>
-      </c>
-      <c r="F130" s="13">
-        <v>4.3945299999999996</v>
-      </c>
-      <c r="G130" s="12">
-        <v>448</v>
-      </c>
-      <c r="H130" s="13">
-        <v>1.6419999999999999</v>
-      </c>
-      <c r="I130" s="14">
-        <v>1.63923</v>
+      <c r="D130" s="22">
+        <v>172</v>
+      </c>
+      <c r="E130" s="23">
+        <v>4.0687199999999999</v>
+      </c>
+      <c r="F130" s="23">
+        <v>4.0879399999999997</v>
+      </c>
+      <c r="G130" s="22">
+        <v>345</v>
+      </c>
+      <c r="H130" s="23">
+        <v>2.6093000000000002</v>
+      </c>
+      <c r="I130" s="24">
+        <v>2.6268099999999999</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>9</v>
@@ -11162,14 +11165,14 @@
     </row>
     <row r="132" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C132" s="6"/>
-      <c r="D132" s="38" t="s">
+      <c r="D132" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E132" s="38"/>
-      <c r="F132" s="38"/>
-      <c r="G132" s="38"/>
-      <c r="H132" s="38"/>
-      <c r="I132" s="39"/>
+      <c r="E132" s="36"/>
+      <c r="F132" s="36"/>
+      <c r="G132" s="36"/>
+      <c r="H132" s="36"/>
+      <c r="I132" s="37"/>
       <c r="L132" s="1" t="s">
         <v>89</v>
       </c>
@@ -11242,16 +11245,16 @@
     </row>
     <row r="133" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C133" s="7"/>
-      <c r="D133" s="36" t="s">
+      <c r="D133" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E133" s="36"/>
-      <c r="F133" s="36"/>
-      <c r="G133" s="36" t="s">
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H133" s="36"/>
-      <c r="I133" s="37"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="39"/>
       <c r="L133" s="1" t="s">
         <v>90</v>
       </c>
@@ -11563,7 +11566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="3:40" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:40" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C137" s="18" t="s">
         <v>140</v>
       </c>
@@ -11655,7 +11658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="3:40" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:40" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C138" s="18" t="s">
         <v>141</v>
       </c>
@@ -11784,7 +11787,7 @@
         <v>3.6098400000000003E-2</v>
       </c>
     </row>
-    <row r="141" spans="3:40" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:40" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C141" s="18" t="s">
         <v>140</v>
       </c>
@@ -11807,7 +11810,7 @@
         <v>1.8833900000000001E-2</v>
       </c>
     </row>
-    <row r="142" spans="3:40" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:40" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C142" s="18" t="s">
         <v>141</v>
       </c>
@@ -11864,7 +11867,7 @@
         <v>1.0498000000000001</v>
       </c>
     </row>
-    <row r="145" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C145" s="18" t="s">
         <v>140</v>
       </c>
@@ -11887,7 +11890,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="146" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C146" s="18" t="s">
         <v>141</v>
       </c>
@@ -11912,27 +11915,27 @@
     </row>
     <row r="147" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C147" s="18"/>
-      <c r="D147" s="36" t="s">
+      <c r="D147" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E147" s="36"/>
-      <c r="F147" s="36"/>
-      <c r="G147" s="36"/>
-      <c r="H147" s="36"/>
-      <c r="I147" s="37"/>
+      <c r="E147" s="38"/>
+      <c r="F147" s="38"/>
+      <c r="G147" s="38"/>
+      <c r="H147" s="38"/>
+      <c r="I147" s="39"/>
     </row>
     <row r="148" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C148" s="18"/>
-      <c r="D148" s="36" t="s">
+      <c r="D148" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E148" s="36"/>
-      <c r="F148" s="36"/>
-      <c r="G148" s="36" t="s">
+      <c r="E148" s="38"/>
+      <c r="F148" s="38"/>
+      <c r="G148" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H148" s="36"/>
-      <c r="I148" s="37"/>
+      <c r="H148" s="38"/>
+      <c r="I148" s="39"/>
     </row>
     <row r="149" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C149" s="18"/>
@@ -11989,7 +11992,7 @@
         <v>2.3437499999999999E-3</v>
       </c>
     </row>
-    <row r="152" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C152" s="18" t="s">
         <v>140</v>
       </c>
@@ -12012,7 +12015,7 @@
         <v>1.1997799999999999E-3</v>
       </c>
     </row>
-    <row r="153" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C153" s="18" t="s">
         <v>141</v>
       </c>
@@ -12069,7 +12072,7 @@
         <v>3.6900599999999999E-2</v>
       </c>
     </row>
-    <row r="156" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C156" s="18" t="s">
         <v>140</v>
       </c>
@@ -12092,7 +12095,7 @@
         <v>1.9252399999999999E-2</v>
       </c>
     </row>
-    <row r="157" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C157" s="18" t="s">
         <v>141</v>
       </c>
@@ -12149,7 +12152,7 @@
         <v>1.07422</v>
       </c>
     </row>
-    <row r="160" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C160" s="18" t="s">
         <v>140</v>
       </c>
@@ -12176,7 +12179,7 @@
       <c r="S160" s="5"/>
       <c r="T160" s="5"/>
     </row>
-    <row r="161" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C161" s="18" t="s">
         <v>141</v>
       </c>
@@ -12205,14 +12208,14 @@
     </row>
     <row r="162" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C162" s="18"/>
-      <c r="D162" s="36" t="s">
+      <c r="D162" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E162" s="36"/>
-      <c r="F162" s="36"/>
-      <c r="G162" s="36"/>
-      <c r="H162" s="36"/>
-      <c r="I162" s="37"/>
+      <c r="E162" s="38"/>
+      <c r="F162" s="38"/>
+      <c r="G162" s="38"/>
+      <c r="H162" s="38"/>
+      <c r="I162" s="39"/>
       <c r="N162" s="5"/>
       <c r="O162" s="5"/>
       <c r="S162" s="5"/>
@@ -12220,16 +12223,16 @@
     </row>
     <row r="163" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C163" s="18"/>
-      <c r="D163" s="36" t="s">
+      <c r="D163" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E163" s="36"/>
-      <c r="F163" s="36"/>
-      <c r="G163" s="36" t="s">
+      <c r="E163" s="38"/>
+      <c r="F163" s="38"/>
+      <c r="G163" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H163" s="36"/>
-      <c r="I163" s="37"/>
+      <c r="H163" s="38"/>
+      <c r="I163" s="39"/>
       <c r="N163" s="5"/>
       <c r="O163" s="5"/>
       <c r="S163" s="5"/>
@@ -12302,7 +12305,7 @@
       <c r="S166" s="5"/>
       <c r="T166" s="5"/>
     </row>
-    <row r="167" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C167" s="18" t="s">
         <v>140</v>
       </c>
@@ -12329,7 +12332,7 @@
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
     </row>
-    <row r="168" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C168" s="18" t="s">
         <v>141</v>
       </c>
@@ -12394,7 +12397,7 @@
         <v>3.8504999999999998E-2</v>
       </c>
     </row>
-    <row r="171" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C171" s="18" t="s">
         <v>140</v>
       </c>
@@ -12417,7 +12420,7 @@
         <v>1.81359E-2</v>
       </c>
     </row>
-    <row r="172" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C172" s="18" t="s">
         <v>141</v>
       </c>
@@ -12492,7 +12495,7 @@
       <c r="AB174" s="5"/>
       <c r="AC174" s="5"/>
     </row>
-    <row r="175" spans="3:29" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C175" s="18" t="s">
         <v>140</v>
       </c>
@@ -12521,7 +12524,7 @@
       <c r="AB175" s="5"/>
       <c r="AC175" s="5"/>
     </row>
-    <row r="176" spans="3:29" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:29" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C176" s="18" t="s">
         <v>141</v>
       </c>
@@ -12560,14 +12563,14 @@
     </row>
     <row r="178" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C178" s="25"/>
-      <c r="D178" s="38" t="s">
+      <c r="D178" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E178" s="38"/>
-      <c r="F178" s="38"/>
-      <c r="G178" s="38"/>
-      <c r="H178" s="38"/>
-      <c r="I178" s="39"/>
+      <c r="E178" s="36"/>
+      <c r="F178" s="36"/>
+      <c r="G178" s="36"/>
+      <c r="H178" s="36"/>
+      <c r="I178" s="37"/>
       <c r="R178" s="5"/>
       <c r="S178" s="5"/>
       <c r="W178" s="5"/>
@@ -12577,16 +12580,16 @@
     </row>
     <row r="179" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C179" s="26"/>
-      <c r="D179" s="36" t="s">
+      <c r="D179" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E179" s="36"/>
-      <c r="F179" s="36"/>
-      <c r="G179" s="36" t="s">
+      <c r="E179" s="38"/>
+      <c r="F179" s="38"/>
+      <c r="G179" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H179" s="36"/>
-      <c r="I179" s="37"/>
+      <c r="H179" s="38"/>
+      <c r="I179" s="39"/>
       <c r="R179" s="5"/>
       <c r="S179" s="5"/>
       <c r="W179" s="5"/>
@@ -12886,28 +12889,28 @@
     </row>
     <row r="191" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C191" s="7"/>
-      <c r="D191" s="36" t="s">
+      <c r="D191" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E191" s="36"/>
-      <c r="F191" s="36"/>
-      <c r="G191" s="36"/>
-      <c r="H191" s="36"/>
-      <c r="I191" s="37"/>
+      <c r="E191" s="38"/>
+      <c r="F191" s="38"/>
+      <c r="G191" s="38"/>
+      <c r="H191" s="38"/>
+      <c r="I191" s="39"/>
       <c r="R191" s="5"/>
     </row>
     <row r="192" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C192" s="7"/>
-      <c r="D192" s="36" t="s">
+      <c r="D192" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E192" s="36"/>
-      <c r="F192" s="36"/>
-      <c r="G192" s="36" t="s">
+      <c r="E192" s="38"/>
+      <c r="F192" s="38"/>
+      <c r="G192" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H192" s="36"/>
-      <c r="I192" s="37"/>
+      <c r="H192" s="38"/>
+      <c r="I192" s="39"/>
       <c r="R192" s="5"/>
     </row>
     <row r="193" spans="3:30" ht="31.2" x14ac:dyDescent="0.3">
@@ -13163,27 +13166,27 @@
     </row>
     <row r="204" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C204" s="18"/>
-      <c r="D204" s="36" t="s">
+      <c r="D204" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E204" s="36"/>
-      <c r="F204" s="36"/>
-      <c r="G204" s="36"/>
-      <c r="H204" s="36"/>
-      <c r="I204" s="37"/>
+      <c r="E204" s="38"/>
+      <c r="F204" s="38"/>
+      <c r="G204" s="38"/>
+      <c r="H204" s="38"/>
+      <c r="I204" s="39"/>
     </row>
     <row r="205" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C205" s="18"/>
-      <c r="D205" s="36" t="s">
+      <c r="D205" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E205" s="36"/>
-      <c r="F205" s="36"/>
-      <c r="G205" s="36" t="s">
+      <c r="E205" s="38"/>
+      <c r="F205" s="38"/>
+      <c r="G205" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H205" s="36"/>
-      <c r="I205" s="37"/>
+      <c r="H205" s="38"/>
+      <c r="I205" s="39"/>
     </row>
     <row r="206" spans="3:30" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C206" s="18"/>
@@ -13474,29 +13477,29 @@
     </row>
     <row r="221" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C221" s="25"/>
-      <c r="D221" s="38" t="s">
+      <c r="D221" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E221" s="38"/>
-      <c r="F221" s="38"/>
-      <c r="G221" s="38"/>
-      <c r="H221" s="38"/>
-      <c r="I221" s="39"/>
+      <c r="E221" s="36"/>
+      <c r="F221" s="36"/>
+      <c r="G221" s="36"/>
+      <c r="H221" s="36"/>
+      <c r="I221" s="37"/>
       <c r="N221" s="5"/>
       <c r="O221" s="5"/>
     </row>
     <row r="222" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C222" s="26"/>
-      <c r="D222" s="36" t="s">
+      <c r="D222" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E222" s="36"/>
-      <c r="F222" s="36"/>
-      <c r="G222" s="36" t="s">
+      <c r="E222" s="38"/>
+      <c r="F222" s="38"/>
+      <c r="G222" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H222" s="36"/>
-      <c r="I222" s="37"/>
+      <c r="H222" s="38"/>
+      <c r="I222" s="39"/>
       <c r="N222" s="5"/>
       <c r="O222" s="5"/>
     </row>
@@ -13663,27 +13666,27 @@
     </row>
     <row r="230" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C230" s="7"/>
-      <c r="D230" s="36" t="s">
+      <c r="D230" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E230" s="36"/>
-      <c r="F230" s="36"/>
-      <c r="G230" s="36"/>
-      <c r="H230" s="36"/>
-      <c r="I230" s="37"/>
+      <c r="E230" s="38"/>
+      <c r="F230" s="38"/>
+      <c r="G230" s="38"/>
+      <c r="H230" s="38"/>
+      <c r="I230" s="39"/>
     </row>
     <row r="231" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C231" s="7"/>
-      <c r="D231" s="36" t="s">
+      <c r="D231" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E231" s="36"/>
-      <c r="F231" s="36"/>
-      <c r="G231" s="36" t="s">
+      <c r="E231" s="38"/>
+      <c r="F231" s="38"/>
+      <c r="G231" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H231" s="36"/>
-      <c r="I231" s="37"/>
+      <c r="H231" s="38"/>
+      <c r="I231" s="39"/>
     </row>
     <row r="232" spans="3:30" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C232" s="7"/>
@@ -13852,29 +13855,29 @@
     </row>
     <row r="239" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C239" s="18"/>
-      <c r="D239" s="36" t="s">
+      <c r="D239" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E239" s="36"/>
-      <c r="F239" s="36"/>
-      <c r="G239" s="36"/>
-      <c r="H239" s="36"/>
-      <c r="I239" s="37"/>
+      <c r="E239" s="38"/>
+      <c r="F239" s="38"/>
+      <c r="G239" s="38"/>
+      <c r="H239" s="38"/>
+      <c r="I239" s="39"/>
       <c r="AC239" s="5"/>
       <c r="AD239" s="5"/>
     </row>
     <row r="240" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C240" s="18"/>
-      <c r="D240" s="36" t="s">
+      <c r="D240" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E240" s="36"/>
-      <c r="F240" s="36"/>
-      <c r="G240" s="36" t="s">
+      <c r="E240" s="38"/>
+      <c r="F240" s="38"/>
+      <c r="G240" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H240" s="36"/>
-      <c r="I240" s="37"/>
+      <c r="H240" s="38"/>
+      <c r="I240" s="39"/>
       <c r="AC240" s="5"/>
       <c r="AD240" s="5"/>
     </row>
@@ -14046,27 +14049,27 @@
     <row r="248" spans="3:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="249" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C249" s="25"/>
-      <c r="D249" s="38" t="s">
+      <c r="D249" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E249" s="38"/>
-      <c r="F249" s="38"/>
-      <c r="G249" s="38"/>
-      <c r="H249" s="38"/>
-      <c r="I249" s="39"/>
+      <c r="E249" s="36"/>
+      <c r="F249" s="36"/>
+      <c r="G249" s="36"/>
+      <c r="H249" s="36"/>
+      <c r="I249" s="37"/>
     </row>
     <row r="250" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C250" s="26"/>
-      <c r="D250" s="36" t="s">
+      <c r="D250" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E250" s="36"/>
-      <c r="F250" s="36"/>
-      <c r="G250" s="36" t="s">
+      <c r="E250" s="38"/>
+      <c r="F250" s="38"/>
+      <c r="G250" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H250" s="36"/>
-      <c r="I250" s="37"/>
+      <c r="H250" s="38"/>
+      <c r="I250" s="39"/>
     </row>
     <row r="251" spans="3:30" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C251" s="26"/>
@@ -14262,27 +14265,27 @@
     </row>
     <row r="261" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C261" s="7"/>
-      <c r="D261" s="36" t="s">
+      <c r="D261" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E261" s="36"/>
-      <c r="F261" s="36"/>
-      <c r="G261" s="36"/>
-      <c r="H261" s="36"/>
-      <c r="I261" s="37"/>
+      <c r="E261" s="38"/>
+      <c r="F261" s="38"/>
+      <c r="G261" s="38"/>
+      <c r="H261" s="38"/>
+      <c r="I261" s="39"/>
     </row>
     <row r="262" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C262" s="7"/>
-      <c r="D262" s="36" t="s">
+      <c r="D262" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E262" s="36"/>
-      <c r="F262" s="36"/>
-      <c r="G262" s="36" t="s">
+      <c r="E262" s="38"/>
+      <c r="F262" s="38"/>
+      <c r="G262" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H262" s="36"/>
-      <c r="I262" s="37"/>
+      <c r="H262" s="38"/>
+      <c r="I262" s="39"/>
     </row>
     <row r="263" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C263" s="7"/>
@@ -14490,30 +14493,30 @@
     </row>
     <row r="273" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C273" s="18"/>
-      <c r="D273" s="36" t="s">
+      <c r="D273" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E273" s="36"/>
-      <c r="F273" s="36"/>
-      <c r="G273" s="36"/>
-      <c r="H273" s="36"/>
-      <c r="I273" s="37"/>
+      <c r="E273" s="38"/>
+      <c r="F273" s="38"/>
+      <c r="G273" s="38"/>
+      <c r="H273" s="38"/>
+      <c r="I273" s="39"/>
       <c r="R273" s="5"/>
       <c r="AB273" s="5"/>
       <c r="AC273" s="5"/>
     </row>
     <row r="274" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C274" s="18"/>
-      <c r="D274" s="36" t="s">
+      <c r="D274" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E274" s="36"/>
-      <c r="F274" s="36"/>
-      <c r="G274" s="36" t="s">
+      <c r="E274" s="38"/>
+      <c r="F274" s="38"/>
+      <c r="G274" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H274" s="36"/>
-      <c r="I274" s="37"/>
+      <c r="H274" s="38"/>
+      <c r="I274" s="39"/>
       <c r="R274" s="5"/>
       <c r="AB274" s="5"/>
       <c r="AC274" s="5"/>
@@ -14729,28 +14732,28 @@
     </row>
     <row r="286" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C286" s="25"/>
-      <c r="D286" s="38" t="s">
+      <c r="D286" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E286" s="38"/>
-      <c r="F286" s="38"/>
-      <c r="G286" s="38"/>
-      <c r="H286" s="38"/>
-      <c r="I286" s="39"/>
+      <c r="E286" s="36"/>
+      <c r="F286" s="36"/>
+      <c r="G286" s="36"/>
+      <c r="H286" s="36"/>
+      <c r="I286" s="37"/>
       <c r="R286" s="5"/>
     </row>
     <row r="287" spans="3:29" x14ac:dyDescent="0.3">
       <c r="C287" s="26"/>
-      <c r="D287" s="36" t="s">
+      <c r="D287" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E287" s="36"/>
-      <c r="F287" s="36"/>
-      <c r="G287" s="36" t="s">
+      <c r="E287" s="38"/>
+      <c r="F287" s="38"/>
+      <c r="G287" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H287" s="36"/>
-      <c r="I287" s="37"/>
+      <c r="H287" s="38"/>
+      <c r="I287" s="39"/>
       <c r="R287" s="5"/>
     </row>
     <row r="288" spans="3:29" ht="31.2" x14ac:dyDescent="0.3">
@@ -14947,27 +14950,27 @@
     </row>
     <row r="298" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C298" s="7"/>
-      <c r="D298" s="36" t="s">
+      <c r="D298" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E298" s="36"/>
-      <c r="F298" s="36"/>
-      <c r="G298" s="36"/>
-      <c r="H298" s="36"/>
-      <c r="I298" s="37"/>
+      <c r="E298" s="38"/>
+      <c r="F298" s="38"/>
+      <c r="G298" s="38"/>
+      <c r="H298" s="38"/>
+      <c r="I298" s="39"/>
     </row>
     <row r="299" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C299" s="7"/>
-      <c r="D299" s="36" t="s">
+      <c r="D299" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E299" s="36"/>
-      <c r="F299" s="36"/>
-      <c r="G299" s="36" t="s">
+      <c r="E299" s="38"/>
+      <c r="F299" s="38"/>
+      <c r="G299" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H299" s="36"/>
-      <c r="I299" s="37"/>
+      <c r="H299" s="38"/>
+      <c r="I299" s="39"/>
     </row>
     <row r="300" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C300" s="7"/>
@@ -15187,30 +15190,30 @@
     </row>
     <row r="310" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C310" s="18"/>
-      <c r="D310" s="36" t="s">
+      <c r="D310" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E310" s="36"/>
-      <c r="F310" s="36"/>
-      <c r="G310" s="36"/>
-      <c r="H310" s="36"/>
-      <c r="I310" s="37"/>
+      <c r="E310" s="38"/>
+      <c r="F310" s="38"/>
+      <c r="G310" s="38"/>
+      <c r="H310" s="38"/>
+      <c r="I310" s="39"/>
       <c r="R310" s="5"/>
       <c r="AB310" s="5"/>
       <c r="AC310" s="5"/>
     </row>
     <row r="311" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C311" s="18"/>
-      <c r="D311" s="36" t="s">
+      <c r="D311" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E311" s="36"/>
-      <c r="F311" s="36"/>
-      <c r="G311" s="36" t="s">
+      <c r="E311" s="38"/>
+      <c r="F311" s="38"/>
+      <c r="G311" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H311" s="36"/>
-      <c r="I311" s="37"/>
+      <c r="H311" s="38"/>
+      <c r="I311" s="39"/>
       <c r="R311" s="5"/>
       <c r="AB311" s="5"/>
       <c r="AC311" s="5"/>
@@ -15434,28 +15437,28 @@
     </row>
     <row r="323" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C323" s="25"/>
-      <c r="D323" s="38" t="s">
+      <c r="D323" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E323" s="38"/>
-      <c r="F323" s="38"/>
-      <c r="G323" s="38"/>
-      <c r="H323" s="38"/>
-      <c r="I323" s="39"/>
+      <c r="E323" s="36"/>
+      <c r="F323" s="36"/>
+      <c r="G323" s="36"/>
+      <c r="H323" s="36"/>
+      <c r="I323" s="37"/>
       <c r="R323" s="5"/>
     </row>
     <row r="324" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C324" s="26"/>
-      <c r="D324" s="36" t="s">
+      <c r="D324" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E324" s="36"/>
-      <c r="F324" s="36"/>
-      <c r="G324" s="36" t="s">
+      <c r="E324" s="38"/>
+      <c r="F324" s="38"/>
+      <c r="G324" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H324" s="36"/>
-      <c r="I324" s="37"/>
+      <c r="H324" s="38"/>
+      <c r="I324" s="39"/>
       <c r="R324" s="5"/>
     </row>
     <row r="325" spans="3:18" ht="31.2" x14ac:dyDescent="0.3">
@@ -15654,27 +15657,27 @@
     </row>
     <row r="335" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C335" s="7"/>
-      <c r="D335" s="36" t="s">
+      <c r="D335" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E335" s="36"/>
-      <c r="F335" s="36"/>
-      <c r="G335" s="36"/>
-      <c r="H335" s="36"/>
-      <c r="I335" s="37"/>
+      <c r="E335" s="38"/>
+      <c r="F335" s="38"/>
+      <c r="G335" s="38"/>
+      <c r="H335" s="38"/>
+      <c r="I335" s="39"/>
     </row>
     <row r="336" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C336" s="7"/>
-      <c r="D336" s="36" t="s">
+      <c r="D336" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E336" s="36"/>
-      <c r="F336" s="36"/>
-      <c r="G336" s="36" t="s">
+      <c r="E336" s="38"/>
+      <c r="F336" s="38"/>
+      <c r="G336" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H336" s="36"/>
-      <c r="I336" s="37"/>
+      <c r="H336" s="38"/>
+      <c r="I336" s="39"/>
     </row>
     <row r="337" spans="3:39" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C337" s="7"/>
@@ -15912,14 +15915,14 @@
     </row>
     <row r="347" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C347" s="18"/>
-      <c r="D347" s="36" t="s">
+      <c r="D347" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E347" s="36"/>
-      <c r="F347" s="36"/>
-      <c r="G347" s="36"/>
-      <c r="H347" s="36"/>
-      <c r="I347" s="37"/>
+      <c r="E347" s="38"/>
+      <c r="F347" s="38"/>
+      <c r="G347" s="38"/>
+      <c r="H347" s="38"/>
+      <c r="I347" s="39"/>
       <c r="R347" s="5"/>
       <c r="AB347" s="5"/>
       <c r="AC347" s="5"/>
@@ -15930,16 +15933,16 @@
     </row>
     <row r="348" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C348" s="18"/>
-      <c r="D348" s="36" t="s">
+      <c r="D348" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E348" s="36"/>
-      <c r="F348" s="36"/>
-      <c r="G348" s="36" t="s">
+      <c r="E348" s="38"/>
+      <c r="F348" s="38"/>
+      <c r="G348" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H348" s="36"/>
-      <c r="I348" s="37"/>
+      <c r="H348" s="38"/>
+      <c r="I348" s="39"/>
       <c r="R348" s="5"/>
       <c r="AB348" s="5"/>
       <c r="AC348" s="5"/>
@@ -16218,14 +16221,14 @@
     </row>
     <row r="360" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C360" s="25"/>
-      <c r="D360" s="38" t="s">
+      <c r="D360" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E360" s="38"/>
-      <c r="F360" s="38"/>
-      <c r="G360" s="38"/>
-      <c r="H360" s="38"/>
-      <c r="I360" s="39"/>
+      <c r="E360" s="36"/>
+      <c r="F360" s="36"/>
+      <c r="G360" s="36"/>
+      <c r="H360" s="36"/>
+      <c r="I360" s="37"/>
       <c r="AG360" s="5"/>
       <c r="AH360" s="5"/>
       <c r="AL360" s="5"/>
@@ -16233,16 +16236,16 @@
     </row>
     <row r="361" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C361" s="26"/>
-      <c r="D361" s="36" t="s">
+      <c r="D361" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E361" s="36"/>
-      <c r="F361" s="36"/>
-      <c r="G361" s="36" t="s">
+      <c r="E361" s="38"/>
+      <c r="F361" s="38"/>
+      <c r="G361" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H361" s="36"/>
-      <c r="I361" s="37"/>
+      <c r="H361" s="38"/>
+      <c r="I361" s="39"/>
       <c r="AG361" s="5"/>
       <c r="AH361" s="5"/>
       <c r="AL361" s="5"/>
@@ -16477,28 +16480,28 @@
     </row>
     <row r="372" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C372" s="7"/>
-      <c r="D372" s="36" t="s">
+      <c r="D372" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E372" s="36"/>
-      <c r="F372" s="36"/>
-      <c r="G372" s="36"/>
-      <c r="H372" s="36"/>
-      <c r="I372" s="37"/>
+      <c r="E372" s="38"/>
+      <c r="F372" s="38"/>
+      <c r="G372" s="38"/>
+      <c r="H372" s="38"/>
+      <c r="I372" s="39"/>
       <c r="R372" s="5"/>
     </row>
     <row r="373" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C373" s="7"/>
-      <c r="D373" s="36" t="s">
+      <c r="D373" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E373" s="36"/>
-      <c r="F373" s="36"/>
-      <c r="G373" s="36" t="s">
+      <c r="E373" s="38"/>
+      <c r="F373" s="38"/>
+      <c r="G373" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H373" s="36"/>
-      <c r="I373" s="37"/>
+      <c r="H373" s="38"/>
+      <c r="I373" s="39"/>
       <c r="R373" s="5"/>
     </row>
     <row r="374" spans="3:39" ht="31.2" x14ac:dyDescent="0.3">
@@ -16700,27 +16703,27 @@
     </row>
     <row r="384" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C384" s="18"/>
-      <c r="D384" s="36" t="s">
+      <c r="D384" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E384" s="36"/>
-      <c r="F384" s="36"/>
-      <c r="G384" s="36"/>
-      <c r="H384" s="36"/>
-      <c r="I384" s="37"/>
+      <c r="E384" s="38"/>
+      <c r="F384" s="38"/>
+      <c r="G384" s="38"/>
+      <c r="H384" s="38"/>
+      <c r="I384" s="39"/>
     </row>
     <row r="385" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C385" s="18"/>
-      <c r="D385" s="36" t="s">
+      <c r="D385" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E385" s="36"/>
-      <c r="F385" s="36"/>
-      <c r="G385" s="36" t="s">
+      <c r="E385" s="38"/>
+      <c r="F385" s="38"/>
+      <c r="G385" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H385" s="36"/>
-      <c r="I385" s="37"/>
+      <c r="H385" s="38"/>
+      <c r="I385" s="39"/>
     </row>
     <row r="386" spans="3:39" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C386" s="18"/>
@@ -16945,14 +16948,14 @@
     </row>
     <row r="397" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C397" s="25"/>
-      <c r="D397" s="38" t="s">
+      <c r="D397" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E397" s="38"/>
-      <c r="F397" s="38"/>
-      <c r="G397" s="38"/>
-      <c r="H397" s="38"/>
-      <c r="I397" s="39"/>
+      <c r="E397" s="36"/>
+      <c r="F397" s="36"/>
+      <c r="G397" s="36"/>
+      <c r="H397" s="36"/>
+      <c r="I397" s="37"/>
       <c r="R397" s="5"/>
       <c r="AB397" s="5"/>
       <c r="AC397" s="5"/>
@@ -16963,16 +16966,16 @@
     </row>
     <row r="398" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C398" s="26"/>
-      <c r="D398" s="36" t="s">
+      <c r="D398" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E398" s="36"/>
-      <c r="F398" s="36"/>
-      <c r="G398" s="36" t="s">
+      <c r="E398" s="38"/>
+      <c r="F398" s="38"/>
+      <c r="G398" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H398" s="36"/>
-      <c r="I398" s="37"/>
+      <c r="H398" s="38"/>
+      <c r="I398" s="39"/>
       <c r="R398" s="5"/>
       <c r="AB398" s="5"/>
       <c r="AC398" s="5"/>
@@ -17276,27 +17279,27 @@
     </row>
     <row r="412" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C412" s="7"/>
-      <c r="D412" s="36" t="s">
+      <c r="D412" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E412" s="36"/>
-      <c r="F412" s="36"/>
-      <c r="G412" s="36"/>
-      <c r="H412" s="36"/>
-      <c r="I412" s="37"/>
+      <c r="E412" s="38"/>
+      <c r="F412" s="38"/>
+      <c r="G412" s="38"/>
+      <c r="H412" s="38"/>
+      <c r="I412" s="39"/>
     </row>
     <row r="413" spans="3:39" x14ac:dyDescent="0.3">
       <c r="C413" s="7"/>
-      <c r="D413" s="36" t="s">
+      <c r="D413" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E413" s="36"/>
-      <c r="F413" s="36"/>
-      <c r="G413" s="36" t="s">
+      <c r="E413" s="38"/>
+      <c r="F413" s="38"/>
+      <c r="G413" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H413" s="36"/>
-      <c r="I413" s="37"/>
+      <c r="H413" s="38"/>
+      <c r="I413" s="39"/>
     </row>
     <row r="414" spans="3:39" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C414" s="7"/>
@@ -17561,27 +17564,27 @@
     </row>
     <row r="427" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C427" s="18"/>
-      <c r="D427" s="36" t="s">
+      <c r="D427" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E427" s="36"/>
-      <c r="F427" s="36"/>
-      <c r="G427" s="36"/>
-      <c r="H427" s="36"/>
-      <c r="I427" s="37"/>
+      <c r="E427" s="38"/>
+      <c r="F427" s="38"/>
+      <c r="G427" s="38"/>
+      <c r="H427" s="38"/>
+      <c r="I427" s="39"/>
     </row>
     <row r="428" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C428" s="18"/>
-      <c r="D428" s="36" t="s">
+      <c r="D428" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E428" s="36"/>
-      <c r="F428" s="36"/>
-      <c r="G428" s="36" t="s">
+      <c r="E428" s="38"/>
+      <c r="F428" s="38"/>
+      <c r="G428" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H428" s="36"/>
-      <c r="I428" s="37"/>
+      <c r="H428" s="38"/>
+      <c r="I428" s="39"/>
     </row>
     <row r="429" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C429" s="18"/>
@@ -17847,27 +17850,27 @@
     <row r="442" spans="3:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="443" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C443" s="25"/>
-      <c r="D443" s="38" t="s">
+      <c r="D443" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E443" s="38"/>
-      <c r="F443" s="38"/>
-      <c r="G443" s="38"/>
-      <c r="H443" s="38"/>
-      <c r="I443" s="39"/>
+      <c r="E443" s="36"/>
+      <c r="F443" s="36"/>
+      <c r="G443" s="36"/>
+      <c r="H443" s="36"/>
+      <c r="I443" s="37"/>
     </row>
     <row r="444" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C444" s="26"/>
-      <c r="D444" s="36" t="s">
+      <c r="D444" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E444" s="36"/>
-      <c r="F444" s="36"/>
-      <c r="G444" s="36" t="s">
+      <c r="E444" s="38"/>
+      <c r="F444" s="38"/>
+      <c r="G444" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H444" s="36"/>
-      <c r="I444" s="37"/>
+      <c r="H444" s="38"/>
+      <c r="I444" s="39"/>
     </row>
     <row r="445" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C445" s="7"/>
@@ -17972,27 +17975,27 @@
     </row>
     <row r="450" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C450" s="7"/>
-      <c r="D450" s="36" t="s">
+      <c r="D450" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E450" s="36"/>
-      <c r="F450" s="36"/>
-      <c r="G450" s="36"/>
-      <c r="H450" s="36"/>
-      <c r="I450" s="37"/>
+      <c r="E450" s="38"/>
+      <c r="F450" s="38"/>
+      <c r="G450" s="38"/>
+      <c r="H450" s="38"/>
+      <c r="I450" s="39"/>
     </row>
     <row r="451" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C451" s="7"/>
-      <c r="D451" s="36" t="s">
+      <c r="D451" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E451" s="36"/>
-      <c r="F451" s="36"/>
-      <c r="G451" s="36" t="s">
+      <c r="E451" s="38"/>
+      <c r="F451" s="38"/>
+      <c r="G451" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H451" s="36"/>
-      <c r="I451" s="37"/>
+      <c r="H451" s="38"/>
+      <c r="I451" s="39"/>
     </row>
     <row r="452" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C452" s="7"/>
@@ -18097,27 +18100,27 @@
     </row>
     <row r="457" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C457" s="18"/>
-      <c r="D457" s="36" t="s">
+      <c r="D457" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E457" s="36"/>
-      <c r="F457" s="36"/>
-      <c r="G457" s="36"/>
-      <c r="H457" s="36"/>
-      <c r="I457" s="37"/>
+      <c r="E457" s="38"/>
+      <c r="F457" s="38"/>
+      <c r="G457" s="38"/>
+      <c r="H457" s="38"/>
+      <c r="I457" s="39"/>
     </row>
     <row r="458" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C458" s="18"/>
-      <c r="D458" s="36" t="s">
+      <c r="D458" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E458" s="36"/>
-      <c r="F458" s="36"/>
-      <c r="G458" s="36" t="s">
+      <c r="E458" s="38"/>
+      <c r="F458" s="38"/>
+      <c r="G458" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H458" s="36"/>
-      <c r="I458" s="37"/>
+      <c r="H458" s="38"/>
+      <c r="I458" s="39"/>
     </row>
     <row r="459" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C459" s="18"/>
@@ -18223,27 +18226,27 @@
     <row r="464" spans="3:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="465" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C465" s="25"/>
-      <c r="D465" s="38" t="s">
+      <c r="D465" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E465" s="38"/>
-      <c r="F465" s="38"/>
-      <c r="G465" s="38"/>
-      <c r="H465" s="38"/>
-      <c r="I465" s="39"/>
+      <c r="E465" s="36"/>
+      <c r="F465" s="36"/>
+      <c r="G465" s="36"/>
+      <c r="H465" s="36"/>
+      <c r="I465" s="37"/>
     </row>
     <row r="466" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C466" s="26"/>
-      <c r="D466" s="36" t="s">
+      <c r="D466" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E466" s="36"/>
-      <c r="F466" s="36"/>
-      <c r="G466" s="36" t="s">
+      <c r="E466" s="38"/>
+      <c r="F466" s="38"/>
+      <c r="G466" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H466" s="36"/>
-      <c r="I466" s="37"/>
+      <c r="H466" s="38"/>
+      <c r="I466" s="39"/>
     </row>
     <row r="467" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C467" s="7"/>
@@ -18325,27 +18328,27 @@
     </row>
     <row r="471" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C471" s="7"/>
-      <c r="D471" s="36" t="s">
+      <c r="D471" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E471" s="36"/>
-      <c r="F471" s="36"/>
-      <c r="G471" s="36"/>
-      <c r="H471" s="36"/>
-      <c r="I471" s="37"/>
+      <c r="E471" s="38"/>
+      <c r="F471" s="38"/>
+      <c r="G471" s="38"/>
+      <c r="H471" s="38"/>
+      <c r="I471" s="39"/>
     </row>
     <row r="472" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C472" s="7"/>
-      <c r="D472" s="36" t="s">
+      <c r="D472" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E472" s="36"/>
-      <c r="F472" s="36"/>
-      <c r="G472" s="36" t="s">
+      <c r="E472" s="38"/>
+      <c r="F472" s="38"/>
+      <c r="G472" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H472" s="36"/>
-      <c r="I472" s="37"/>
+      <c r="H472" s="38"/>
+      <c r="I472" s="39"/>
     </row>
     <row r="473" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C473" s="7"/>
@@ -18427,27 +18430,27 @@
     </row>
     <row r="477" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C477" s="18"/>
-      <c r="D477" s="36" t="s">
+      <c r="D477" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E477" s="36"/>
-      <c r="F477" s="36"/>
-      <c r="G477" s="36"/>
-      <c r="H477" s="36"/>
-      <c r="I477" s="37"/>
+      <c r="E477" s="38"/>
+      <c r="F477" s="38"/>
+      <c r="G477" s="38"/>
+      <c r="H477" s="38"/>
+      <c r="I477" s="39"/>
     </row>
     <row r="478" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C478" s="18"/>
-      <c r="D478" s="36" t="s">
+      <c r="D478" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E478" s="36"/>
-      <c r="F478" s="36"/>
-      <c r="G478" s="36" t="s">
+      <c r="E478" s="38"/>
+      <c r="F478" s="38"/>
+      <c r="G478" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H478" s="36"/>
-      <c r="I478" s="37"/>
+      <c r="H478" s="38"/>
+      <c r="I478" s="39"/>
     </row>
     <row r="479" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C479" s="18"/>
@@ -18529,10 +18532,10 @@
     </row>
   </sheetData>
   <mergeCells count="201">
-    <mergeCell ref="D428:F428"/>
-    <mergeCell ref="G428:I428"/>
-    <mergeCell ref="D446:I446"/>
-    <mergeCell ref="D471:I471"/>
+    <mergeCell ref="D453:I453"/>
+    <mergeCell ref="D460:I460"/>
+    <mergeCell ref="D468:I468"/>
+    <mergeCell ref="D474:I474"/>
     <mergeCell ref="D472:F472"/>
     <mergeCell ref="G472:I472"/>
     <mergeCell ref="D477:I477"/>
@@ -18544,9 +18547,6 @@
     <mergeCell ref="D465:I465"/>
     <mergeCell ref="D466:F466"/>
     <mergeCell ref="G466:I466"/>
-    <mergeCell ref="D384:I384"/>
-    <mergeCell ref="D385:F385"/>
-    <mergeCell ref="G385:I385"/>
     <mergeCell ref="D397:I397"/>
     <mergeCell ref="D398:F398"/>
     <mergeCell ref="G398:I398"/>
@@ -18561,22 +18561,15 @@
     <mergeCell ref="D390:I390"/>
     <mergeCell ref="D393:I393"/>
     <mergeCell ref="D387:I387"/>
-    <mergeCell ref="D273:I273"/>
-    <mergeCell ref="D274:F274"/>
-    <mergeCell ref="G274:I274"/>
-    <mergeCell ref="D289:I289"/>
-    <mergeCell ref="D292:I292"/>
-    <mergeCell ref="D295:I295"/>
-    <mergeCell ref="D335:I335"/>
-    <mergeCell ref="D336:F336"/>
-    <mergeCell ref="G336:I336"/>
-    <mergeCell ref="D310:I310"/>
-    <mergeCell ref="D311:F311"/>
-    <mergeCell ref="G311:I311"/>
-    <mergeCell ref="D323:I323"/>
-    <mergeCell ref="D324:F324"/>
-    <mergeCell ref="G324:I324"/>
     <mergeCell ref="D326:I326"/>
+    <mergeCell ref="D316:I316"/>
+    <mergeCell ref="D319:I319"/>
+    <mergeCell ref="D298:I298"/>
+    <mergeCell ref="D299:F299"/>
+    <mergeCell ref="G299:I299"/>
+    <mergeCell ref="D384:I384"/>
+    <mergeCell ref="D385:F385"/>
+    <mergeCell ref="G385:I385"/>
     <mergeCell ref="D239:I239"/>
     <mergeCell ref="D240:F240"/>
     <mergeCell ref="G240:I240"/>
@@ -18603,6 +18596,16 @@
     <mergeCell ref="D178:I178"/>
     <mergeCell ref="D125:I125"/>
     <mergeCell ref="D128:I128"/>
+    <mergeCell ref="D132:I132"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="G133:I133"/>
+    <mergeCell ref="D135:I135"/>
+    <mergeCell ref="D139:I139"/>
+    <mergeCell ref="D143:I143"/>
+    <mergeCell ref="D147:I147"/>
+    <mergeCell ref="D148:F148"/>
+    <mergeCell ref="G148:I148"/>
+    <mergeCell ref="D150:I150"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="D78:F78"/>
@@ -18619,6 +18622,7 @@
     <mergeCell ref="D38:I38"/>
     <mergeCell ref="D46:I46"/>
     <mergeCell ref="D53:I53"/>
+    <mergeCell ref="D63:I63"/>
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="D29:I29"/>
     <mergeCell ref="D6:F6"/>
@@ -18632,7 +18636,6 @@
     <mergeCell ref="D20:I20"/>
     <mergeCell ref="D23:I23"/>
     <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D63:I63"/>
     <mergeCell ref="D80:I80"/>
     <mergeCell ref="D70:I70"/>
     <mergeCell ref="D87:I87"/>
@@ -18649,16 +18652,6 @@
     <mergeCell ref="D108:F108"/>
     <mergeCell ref="G108:I108"/>
     <mergeCell ref="D95:I95"/>
-    <mergeCell ref="D132:I132"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="G133:I133"/>
-    <mergeCell ref="D135:I135"/>
-    <mergeCell ref="D139:I139"/>
-    <mergeCell ref="D143:I143"/>
-    <mergeCell ref="D147:I147"/>
-    <mergeCell ref="D148:F148"/>
-    <mergeCell ref="G148:I148"/>
-    <mergeCell ref="D150:I150"/>
     <mergeCell ref="D154:I154"/>
     <mergeCell ref="D158:I158"/>
     <mergeCell ref="D162:I162"/>
@@ -18668,8 +18661,6 @@
     <mergeCell ref="D169:I169"/>
     <mergeCell ref="D173:I173"/>
     <mergeCell ref="D313:I313"/>
-    <mergeCell ref="D316:I316"/>
-    <mergeCell ref="D319:I319"/>
     <mergeCell ref="D301:I301"/>
     <mergeCell ref="D304:I304"/>
     <mergeCell ref="D307:I307"/>
@@ -18685,9 +18676,6 @@
     <mergeCell ref="D286:I286"/>
     <mergeCell ref="D287:F287"/>
     <mergeCell ref="G287:I287"/>
-    <mergeCell ref="D298:I298"/>
-    <mergeCell ref="D299:F299"/>
-    <mergeCell ref="G299:I299"/>
     <mergeCell ref="D261:I261"/>
     <mergeCell ref="D262:F262"/>
     <mergeCell ref="G262:I262"/>
@@ -18697,6 +18685,21 @@
     <mergeCell ref="D353:I353"/>
     <mergeCell ref="D332:I332"/>
     <mergeCell ref="D344:I344"/>
+    <mergeCell ref="D273:I273"/>
+    <mergeCell ref="D274:F274"/>
+    <mergeCell ref="G274:I274"/>
+    <mergeCell ref="D289:I289"/>
+    <mergeCell ref="D292:I292"/>
+    <mergeCell ref="D295:I295"/>
+    <mergeCell ref="D335:I335"/>
+    <mergeCell ref="D336:F336"/>
+    <mergeCell ref="G336:I336"/>
+    <mergeCell ref="D310:I310"/>
+    <mergeCell ref="D311:F311"/>
+    <mergeCell ref="G311:I311"/>
+    <mergeCell ref="D323:I323"/>
+    <mergeCell ref="D324:F324"/>
+    <mergeCell ref="G324:I324"/>
     <mergeCell ref="D356:I356"/>
     <mergeCell ref="D363:I363"/>
     <mergeCell ref="D375:I375"/>
@@ -18706,10 +18709,6 @@
     <mergeCell ref="D348:F348"/>
     <mergeCell ref="G348:I348"/>
     <mergeCell ref="D338:I338"/>
-    <mergeCell ref="D453:I453"/>
-    <mergeCell ref="D460:I460"/>
-    <mergeCell ref="D468:I468"/>
-    <mergeCell ref="D474:I474"/>
     <mergeCell ref="D480:I480"/>
     <mergeCell ref="D400:I400"/>
     <mergeCell ref="D415:I415"/>
@@ -18730,6 +18729,10 @@
     <mergeCell ref="D413:F413"/>
     <mergeCell ref="G413:I413"/>
     <mergeCell ref="D427:I427"/>
+    <mergeCell ref="D428:F428"/>
+    <mergeCell ref="G428:I428"/>
+    <mergeCell ref="D446:I446"/>
+    <mergeCell ref="D471:I471"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>